<commit_message>
Exercice 2 : jour en français
</commit_message>
<xml_diff>
--- a/exercices/exercice2/ventes_analyse.xlsx
+++ b/exercices/exercice2/ventes_analyse.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Lundi</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Lundi</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Lundi</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Mardi</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Mardi</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Mercredi</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Mercredi</t>
         </is>
       </c>
     </row>
@@ -733,7 +733,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Jeudi</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Jeudi</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Vendredi</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Vendredi</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Samedi</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Samedi</t>
         </is>
       </c>
     </row>
@@ -925,7 +925,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Dimanche</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Dimanche</t>
         </is>
       </c>
     </row>
@@ -972,7 +972,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -983,32 +983,62 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>quantite</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Est</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Non spécifié</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Nord</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Ouest</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Sud</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1023,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1034,12 +1064,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>produit</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>quantite</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Souris</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>38</v>
       </c>
     </row>

</xml_diff>